<commit_message>
waiting for integration with exe
</commit_message>
<xml_diff>
--- a/bugs.xlsx
+++ b/bugs.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="To fix" sheetId="1" r:id="rId1"/>
+    <sheet name="to Implement" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>load schools from db during the registration</t>
   </si>
@@ -42,6 +43,12 @@
   </si>
   <si>
     <t>to be able to add exe such as: fractions</t>
+  </si>
+  <si>
+    <t>remove the requirement of four wrong answers. One should be enough to save the exercise.</t>
+  </si>
+  <si>
+    <t>assiginments: to allow a teacher to create new assignments</t>
   </si>
 </sst>
 </file>
@@ -393,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,6 +441,31 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
recording audit post exe
</commit_message>
<xml_diff>
--- a/bugs.xlsx
+++ b/bugs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="To fix" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>load schools from db during the registration</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>assiginments: to allow a teacher to create new assignments</t>
+  </si>
+  <si>
+    <t>reloading the page with an loaded exercise should reload the list of assignments page.</t>
+  </si>
+  <si>
+    <t>disable check answer when nothing is selected yet.</t>
+  </si>
+  <si>
+    <t>the right answer is always first. Needs to be fixed.</t>
   </si>
 </sst>
 </file>
@@ -400,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,6 +455,21 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -455,7 +479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Go back to older version
</commit_message>
<xml_diff>
--- a/bugs.xlsx
+++ b/bugs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyStuff\FunMath\App\Source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ido\Work\Git\SourceCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,9 @@
     <sheet name="To fix" sheetId="1" r:id="rId1"/>
     <sheet name="to Implement" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To fix'!$A$1:$B$1</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>load schools from db during the registration</t>
   </si>
@@ -58,6 +61,24 @@
   </si>
   <si>
     <t>the right answer is always first. Needs to be fixed.</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Bug/Feature</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -93,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,68 +431,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="85.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Split the "assignment" screen to seperate wells
</commit_message>
<xml_diff>
--- a/bugs.xlsx
+++ b/bugs.xlsx
@@ -16,7 +16,7 @@
     <sheet name="to Implement" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To fix'!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To fix'!$A$1:$B$11</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -431,10 +431,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +451,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -458,7 +459,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -482,7 +483,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -498,7 +499,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -514,24 +515,31 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1"/>
+  <autoFilter ref="A1:B11">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="?"/>
+        <filter val="Open"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
commit latest bugs list
</commit_message>
<xml_diff>
--- a/bugs.xlsx
+++ b/bugs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="To fix" sheetId="1" r:id="rId1"/>
@@ -423,13 +423,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="90.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -491,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>